<commit_message>
Updated the timestep + began working on new calibration
</commit_message>
<xml_diff>
--- a/syphilis_neg_databook_v01_2.xlsx
+++ b/syphilis_neg_databook_v01_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamph\Google Drive (phillip.luong@burnet.edu.au)\Coding Projects\2021-03 Syphilis Modelling Atomica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamph\Documents\GitHub\Syphilis-Atomica-Modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8860473-8085-4249-9EA6-CC659C25CC0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41E3B63-EDE4-4CE5-A796-B7E1001920B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4872" yWindow="5748" windowWidth="12288" windowHeight="6180" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -710,7 +710,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
@@ -754,8 +754,8 @@
   </sheetPr>
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1016,10 +1016,10 @@
   <sheetPr>
     <tabColor rgb="FF808080"/>
   </sheetPr>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,652 +1273,653 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P10" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2020</v>
+      </c>
+    </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I11" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J11" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K11" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L11" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M11" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N11" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O11" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P11" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="str">
+      <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>neg</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
         <v>0.05</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N13" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P13" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>2020</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H14" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I14" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J14" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K14" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L14" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M14" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N14" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O14" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P14" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="str">
+      <c r="A14" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>neg</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
         <v>0.01</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M16" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N16" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O16" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P16" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>2020</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H17" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I17" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J17" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K17" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L17" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M17" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N17" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O17" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P17" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="str">
+      <c r="A17" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>neg</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3">
         <v>0.6</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L19" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M19" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P19" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>2020</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H20" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I20" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J20" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K20" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L20" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M20" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N20" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O20" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P20" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="str">
+      <c r="A20" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>neg</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3">
+        <f>365.25/7</f>
         <v>52.178571428571431</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J22" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K22" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L22" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M22" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N22" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O22" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P22" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>2020</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H23" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I23" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J23" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K23" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L23" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M23" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N23" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O23" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P23" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="str">
+      <c r="A23" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>neg</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3">
         <v>0.4</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J25" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K25" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L25" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M25" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O25" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P25" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>2020</v>
+      </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H26" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I26" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J26" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K26" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L26" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M26" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N26" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O26" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P26" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="str">
+      <c r="A26" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>neg</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C26" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3">
         <v>0.7</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J28" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K28" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L28" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M28" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N28" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O28" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P28" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>2020</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I29" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J29" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K29" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L29" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M29" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N29" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O29" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P29" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="str">
+      <c r="A29" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>neg</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B29" t="s">
         <v>17</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C29" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3">
         <v>0.69</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2011</v>
+      </c>
+      <c r="I31" s="1">
+        <v>2012</v>
+      </c>
+      <c r="J31" s="1">
+        <v>2013</v>
+      </c>
+      <c r="K31" s="1">
+        <v>2014</v>
+      </c>
+      <c r="L31" s="1">
+        <v>2015</v>
+      </c>
+      <c r="M31" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N31" s="1">
+        <v>2017</v>
+      </c>
+      <c r="O31" s="1">
+        <v>2018</v>
+      </c>
+      <c r="P31" s="1">
+        <v>2019</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>2020</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1">
-        <v>2010</v>
-      </c>
-      <c r="H32" s="1">
-        <v>2011</v>
-      </c>
-      <c r="I32" s="1">
-        <v>2012</v>
-      </c>
-      <c r="J32" s="1">
-        <v>2013</v>
-      </c>
-      <c r="K32" s="1">
-        <v>2014</v>
-      </c>
-      <c r="L32" s="1">
-        <v>2015</v>
-      </c>
-      <c r="M32" s="1">
-        <v>2016</v>
-      </c>
-      <c r="N32" s="1">
-        <v>2017</v>
-      </c>
-      <c r="O32" s="1">
-        <v>2018</v>
-      </c>
-      <c r="P32" s="1">
-        <v>2019</v>
-      </c>
-      <c r="Q32" s="1">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C32" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3">
         <f>365.25/224</f>
         <v>1.6305803571428572</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E11">
     <cfRule type="expression" dxfId="21" priority="13">
-      <formula>COUNTIF(G12:Q12,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G11:Q11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="20" priority="14">
-      <formula>AND(COUNTIF(G12:Q12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E12)))</formula>
+      <formula>AND(COUNTIF(G11:Q11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="E14">
     <cfRule type="expression" dxfId="19" priority="15">
-      <formula>COUNTIF(G15:Q15,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G14:Q14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="16">
-      <formula>AND(COUNTIF(G15:Q15,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E15)))</formula>
+      <formula>AND(COUNTIF(G14:Q14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
@@ -1929,36 +1930,36 @@
       <formula>AND(COUNTIF(G2:Q2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
+  <conditionalFormatting sqref="E17">
     <cfRule type="expression" dxfId="15" priority="17">
-      <formula>COUNTIF(G18:Q18,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G17:Q17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="14" priority="18">
-      <formula>AND(COUNTIF(G18:Q18,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E18)))</formula>
+      <formula>AND(COUNTIF(G17:Q17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E20">
     <cfRule type="expression" dxfId="13" priority="19">
-      <formula>COUNTIF(G21:Q21,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G20:Q20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="20">
-      <formula>AND(COUNTIF(G21:Q21,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E21)))</formula>
+      <formula>AND(COUNTIF(G20:Q20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E23">
     <cfRule type="expression" dxfId="11" priority="21">
-      <formula>COUNTIF(G24:Q24,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G23:Q23,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="22">
-      <formula>AND(COUNTIF(G24:Q24,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E24)))</formula>
+      <formula>AND(COUNTIF(G23:Q23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
+  <conditionalFormatting sqref="E26">
     <cfRule type="expression" dxfId="9" priority="23">
-      <formula>COUNTIF(G27:Q27,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G26:Q26,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="24">
-      <formula>AND(COUNTIF(G27:Q27,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E27)))</formula>
+      <formula>AND(COUNTIF(G26:Q26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
@@ -1977,33 +1978,33 @@
       <formula>AND(COUNTIF(G8:Q8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E29">
     <cfRule type="expression" dxfId="3" priority="3">
-      <formula>COUNTIF(G30:Q30,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G29:Q29,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(COUNTIF(G30:Q30,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E30)))</formula>
+      <formula>AND(COUNTIF(G29:Q29,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
+  <conditionalFormatting sqref="E32">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>COUNTIF(G33:Q33,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G32:Q32,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(COUNTIF(G33:Q33,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E33)))</formula>
+      <formula>AND(COUNTIF(G32:Q32,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Number (per year)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C21 C12 C8" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C20 C11 C8" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Rate (per year)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"rate"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18 C27 C24 C30" xr:uid="{00000000-0002-0000-0200-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17 C26 C23 C29" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"probability"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>